<commit_message>
implemented parallel processing, generated results from 5 models on 1000 rows
</commit_message>
<xml_diff>
--- a/sample_outputs/sample_model_comparison_parallel.xlsx
+++ b/sample_outputs/sample_model_comparison_parallel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,6 +455,11 @@
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>hf_distilbert_experience</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>groq_experience</t>
         </is>
@@ -519,6 +524,11 @@
         </is>
       </c>
       <c r="E2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
         <is>
           <t>5 years</t>
         </is>
@@ -577,6 +587,11 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
+          <t>4+</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>4 years</t>
         </is>
       </c>
@@ -620,6 +635,11 @@
         </is>
       </c>
       <c r="E4" t="inlineStr">
+        <is>
+          <t>Not mentioned</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
         <is>
           <t>Not mentioned</t>
         </is>
@@ -676,6 +696,11 @@
           <t>Not mentioned</t>
         </is>
       </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Not mentioned</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -736,6 +761,11 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
+          <t>¬ 1.000</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
           <t>Not mentioned</t>
         </is>
       </c>
@@ -778,6 +808,11 @@
           <t>Not mentioned</t>
         </is>
       </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Not mentioned</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -843,6 +878,11 @@
         </is>
       </c>
       <c r="E8" t="inlineStr">
+        <is>
+          <t>69 96876-224</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
         <is>
           <t>Not mentioned</t>
         </is>
@@ -919,7 +959,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>5 years</t>
+          <t>Not mentioned</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Proven experience as an IT Infrastructure Engineer or in</t>
         </is>
       </c>
     </row>
@@ -1062,6 +1107,11 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
+          <t>10+</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
           <t>10 years</t>
         </is>
       </c>
@@ -1116,6 +1166,11 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
+          <t>Between 4 and 6</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
           <t>4-6 years</t>
         </is>
       </c>
@@ -1172,6 +1227,11 @@
           <t>Not mentioned</t>
         </is>
       </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Not mentioned</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1238,6 +1298,11 @@
         </is>
       </c>
       <c r="E13" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
         <is>
           <t>3 years</t>
         </is>
@@ -1292,6 +1357,11 @@
         </is>
       </c>
       <c r="E14" t="inlineStr">
+        <is>
+          <t>Not mentioned</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
         <is>
           <t>Not mentioned</t>
         </is>
@@ -1358,6 +1428,11 @@
           <t>10 years</t>
         </is>
       </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>10 years</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1448,6 +1523,11 @@
         </is>
       </c>
       <c r="E16" t="inlineStr">
+        <is>
+          <t>13+</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
         <is>
           <t>13 years</t>
         </is>
@@ -1554,6 +1634,11 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
+          <t>18059</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
           <t>Not mentioned</t>
         </is>
       </c>
@@ -1630,7 +1715,12 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>5 years</t>
+          <t>Not mentioned</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Proven experience as an SAP Consultant or in a</t>
         </is>
       </c>
     </row>
@@ -1671,6 +1761,11 @@
         </is>
       </c>
       <c r="E19" t="inlineStr">
+        <is>
+          <t>5 years</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
         <is>
           <t>2 to 5 years</t>
         </is>
@@ -1738,6 +1833,11 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
+          <t>28,000+</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
           <t>Not mentioned</t>
         </is>
       </c>
@@ -1786,6 +1886,11 @@
           <t>Not mentioned</t>
         </is>
       </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Not mentioned</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>